<commit_message>
Updated camera_ttc_euclidean_median.xlsx with more data
</commit_message>
<xml_diff>
--- a/Camera/3D_Object_Tracking/docs/camera_ttc_euclidean_median.xlsx
+++ b/Camera/3D_Object_Tracking/docs/camera_ttc_euclidean_median.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\udacity-sensor-fusion\Camera\3D_Object_Tracking\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08DF07AC-0666-4FCC-9653-F7EFBA614FE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC750120-4955-423A-B0F1-CBF246CB39EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{3E0841BB-29E4-42F0-B515-E8D6117A1835}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{3E0841BB-29E4-42F0-B515-E8D6117A1835}"/>
   </bookViews>
   <sheets>
     <sheet name="18 Frames" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
   <si>
     <t>Frame</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>Within 1.0 of Median</t>
+  </si>
+  <si>
+    <t>Within 2.0 of Median</t>
+  </si>
+  <si>
+    <t>Within 1.5 of Median</t>
   </si>
 </sst>
 </file>
@@ -512,6 +518,324 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-9F31-4B8B-A017-BEF0ACB348CD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'18 Frames'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Within 1.5 of Median</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'18 Frames'!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'18 Frames'!$D$2:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>11.9619</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.607900000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.861999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34.149299999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.2095</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.728199999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.2073</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.650600000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.497</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.500400000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.9816</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.053699999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.819699999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11.0296</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11.7417</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10.474399999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12.605</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-606A-41DB-93E7-CC11C142F491}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'18 Frames'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Within 2.0 of Median</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'18 Frames'!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'18 Frames'!$E$2:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>11.900399999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.3325</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.8032</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.124700000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28.471599999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.2095</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.728199999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.2073</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.650600000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.3644</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.334099999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.9816</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11.981</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.679399999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10.3405</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11.7417</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10.132400000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12.171099999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-606A-41DB-93E7-CC11C142F491}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1946,6 +2270,1032 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-45E6-4C54-A123-D77B649D5EC1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'77 Frames'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Within 1.5 of Median</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'77 Frames'!$A$2:$A$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="77"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>77</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'77 Frames'!$D$2:$D$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="77"/>
+                <c:pt idx="0">
+                  <c:v>11.9619</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.607900000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.861999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34.149299999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.2095</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.728199999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.2073</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.650600000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.497</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.500400000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.9816</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.053699999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.819699999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11.0296</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11.7417</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10.474399999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12.605</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10.0015</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11.045500000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10.745200000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>11.538500000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10.7552</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10.5854</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>10.4765</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>11.3018</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>11.8559</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>10.3094</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>11.5632</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>11.319599999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>14.021100000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>12.622400000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>15.266999999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>11.4579</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>11.7545</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8.38612</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9.0785599999999995</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9.5284399999999998</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9.6067499999999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8.5673899999999996</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>8.4891799999999993</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>9.9578799999999994</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>7.5119199999999999</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>7.8134600000000001</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>8.2756399999999992</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>10.552899999999999</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>10.124499999999999</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>13.583399999999999</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>15.184699999999999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>18.245699999999999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>22.386500000000002</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-375.51900000000001</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-768D-4187-915C-80D4C4334640}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'77 Frames'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Within 2.0 of Median</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'77 Frames'!$A$2:$A$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="77"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>77</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'77 Frames'!$E$2:$E$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="77"/>
+                <c:pt idx="0">
+                  <c:v>11.900399999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.3325</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.8032</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.124700000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28.471599999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.2095</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.728199999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.2073</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.650600000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.3644</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.334099999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.9816</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11.981</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.679399999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10.3405</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11.7417</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10.132400000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12.171099999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10.0015</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11.045500000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10.6233</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>11.538500000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10.628399999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10.2044</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>10.209300000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>10.9115</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>11.511799999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>10.3094</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>11.2189</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>11.4056</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>14.021100000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>12.5595</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>15.266999999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>11.1081</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>11.672800000000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8.41615</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9.1180500000000002</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9.3528599999999997</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9.2371400000000001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>7.7666599999999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7.9642499999999998</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>8.4698399999999996</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>7.0383300000000002</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>7.5830099999999998</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>7.8203800000000001</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>10.209199999999999</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>9.9659999999999993</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>13.629899999999999</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>14.894399999999999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>18.245699999999999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>22.283799999999999</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-375.51900000000001</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-768D-4187-915C-80D4C4334640}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3398,16 +4748,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>19048</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>385762</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>100011</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>252412</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3439,16 +4789,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>157162</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>76198</xdr:rowOff>
+      <xdr:rowOff>109535</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>23812</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:rowOff>166686</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3775,19 +5125,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68843B14-54A3-44F3-89F2-7213B1B1E148}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="11.73046875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3797,8 +5149,14 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3808,8 +5166,14 @@
       <c r="C2">
         <v>11.5556</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D2">
+        <v>11.9619</v>
+      </c>
+      <c r="E2">
+        <v>11.900399999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3819,8 +5183,14 @@
       <c r="C3">
         <v>11.0639</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D3">
+        <v>15.607900000000001</v>
+      </c>
+      <c r="E3">
+        <v>14.3325</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3830,8 +5200,14 @@
       <c r="C4">
         <v>13.2302</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D4">
+        <v>16.861999999999998</v>
+      </c>
+      <c r="E4">
+        <v>13.8032</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3841,8 +5217,14 @@
       <c r="C5">
         <v>13.005699999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D5">
+        <v>13.33</v>
+      </c>
+      <c r="E5">
+        <v>13.124700000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3852,8 +5234,14 @@
       <c r="C6">
         <v>31.424600000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D6">
+        <v>34.149299999999997</v>
+      </c>
+      <c r="E6">
+        <v>28.471599999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3863,8 +5251,14 @@
       <c r="C7">
         <v>38.840800000000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D7">
+        <v>13.2095</v>
+      </c>
+      <c r="E7">
+        <v>13.2095</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3874,8 +5268,14 @@
       <c r="C8">
         <v>7.0369299999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D8">
+        <v>12.728199999999999</v>
+      </c>
+      <c r="E8">
+        <v>12.728199999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3885,8 +5285,14 @@
       <c r="C9">
         <v>11.4003</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D9">
+        <v>12.2073</v>
+      </c>
+      <c r="E9">
+        <v>12.2073</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3896,8 +5302,14 @@
       <c r="C10">
         <v>9.6093299999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D10">
+        <v>12.650600000000001</v>
+      </c>
+      <c r="E10">
+        <v>12.650600000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3907,8 +5319,14 @@
       <c r="C11">
         <v>8.7092700000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D11">
+        <v>13.497</v>
+      </c>
+      <c r="E11">
+        <v>13.3644</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3918,8 +5336,14 @@
       <c r="C12">
         <v>14.4382</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D12">
+        <v>13.500400000000001</v>
+      </c>
+      <c r="E12">
+        <v>13.334099999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3929,8 +5353,14 @@
       <c r="C13">
         <v>8.2389299999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D13">
+        <v>11.9816</v>
+      </c>
+      <c r="E13">
+        <v>11.9816</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3940,8 +5370,14 @@
       <c r="C14">
         <v>11.1959</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D14">
+        <v>12.053699999999999</v>
+      </c>
+      <c r="E14">
+        <v>11.981</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3951,8 +5387,14 @@
       <c r="C15">
         <v>10.6762</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D15">
+        <v>11.819699999999999</v>
+      </c>
+      <c r="E15">
+        <v>11.679399999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3962,8 +5404,14 @@
       <c r="C16">
         <v>7.5277099999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D16">
+        <v>11.0296</v>
+      </c>
+      <c r="E16">
+        <v>10.3405</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3973,8 +5421,14 @@
       <c r="C17">
         <v>10.7415</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D17">
+        <v>11.7417</v>
+      </c>
+      <c r="E17">
+        <v>11.7417</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3984,8 +5438,14 @@
       <c r="C18">
         <v>9.7036300000000004</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D18">
+        <v>10.474399999999999</v>
+      </c>
+      <c r="E18">
+        <v>10.132400000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3995,8 +5455,14 @@
       <c r="C19">
         <v>13.506600000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D19">
+        <v>12.605</v>
+      </c>
+      <c r="E19">
+        <v>12.171099999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -4007,6 +5473,14 @@
       <c r="C21">
         <f>AVERAGE(C2:C19)</f>
         <v>13.439183333333334</v>
+      </c>
+      <c r="D21">
+        <f>AVERAGE(D2:D19)</f>
+        <v>13.96721111111111</v>
+      </c>
+      <c r="E21">
+        <f>AVERAGE(E2:E19)</f>
+        <v>13.286344444444445</v>
       </c>
     </row>
   </sheetData>
@@ -4017,19 +5491,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43C6CF86-4CAB-4D2F-8C85-865E8AC96FFC}">
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T21" sqref="T21"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="10.46484375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4039,8 +5514,14 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4050,8 +5531,14 @@
       <c r="C2">
         <v>11.5556</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D2">
+        <v>11.9619</v>
+      </c>
+      <c r="E2">
+        <v>11.900399999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4061,8 +5548,14 @@
       <c r="C3">
         <v>11.0639</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D3">
+        <v>15.607900000000001</v>
+      </c>
+      <c r="E3">
+        <v>14.3325</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4072,8 +5565,14 @@
       <c r="C4">
         <v>13.2302</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D4">
+        <v>16.861999999999998</v>
+      </c>
+      <c r="E4">
+        <v>13.8032</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4083,8 +5582,14 @@
       <c r="C5">
         <v>13.005699999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D5">
+        <v>13.33</v>
+      </c>
+      <c r="E5">
+        <v>13.124700000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4094,8 +5599,14 @@
       <c r="C6">
         <v>31.424600000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D6">
+        <v>34.149299999999997</v>
+      </c>
+      <c r="E6">
+        <v>28.471599999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4105,8 +5616,14 @@
       <c r="C7">
         <v>38.840800000000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D7">
+        <v>13.2095</v>
+      </c>
+      <c r="E7">
+        <v>13.2095</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4116,8 +5633,14 @@
       <c r="C8">
         <v>7.0369299999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D8">
+        <v>12.728199999999999</v>
+      </c>
+      <c r="E8">
+        <v>12.728199999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4127,8 +5650,14 @@
       <c r="C9">
         <v>11.4003</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D9">
+        <v>12.2073</v>
+      </c>
+      <c r="E9">
+        <v>12.2073</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4138,8 +5667,14 @@
       <c r="C10">
         <v>9.6093299999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D10">
+        <v>12.650600000000001</v>
+      </c>
+      <c r="E10">
+        <v>12.650600000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4149,8 +5684,14 @@
       <c r="C11">
         <v>8.7092700000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D11">
+        <v>13.497</v>
+      </c>
+      <c r="E11">
+        <v>13.3644</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4160,8 +5701,14 @@
       <c r="C12">
         <v>14.4382</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D12">
+        <v>13.500400000000001</v>
+      </c>
+      <c r="E12">
+        <v>13.334099999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4171,8 +5718,14 @@
       <c r="C13">
         <v>8.2389299999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D13">
+        <v>11.9816</v>
+      </c>
+      <c r="E13">
+        <v>11.9816</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4182,8 +5735,14 @@
       <c r="C14">
         <v>11.1959</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D14">
+        <v>12.053699999999999</v>
+      </c>
+      <c r="E14">
+        <v>11.981</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4193,8 +5752,14 @@
       <c r="C15">
         <v>10.6762</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D15">
+        <v>11.819699999999999</v>
+      </c>
+      <c r="E15">
+        <v>11.679399999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4204,8 +5769,14 @@
       <c r="C16">
         <v>7.5277099999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D16">
+        <v>11.0296</v>
+      </c>
+      <c r="E16">
+        <v>10.3405</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4215,8 +5786,14 @@
       <c r="C17">
         <v>10.7415</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D17">
+        <v>11.7417</v>
+      </c>
+      <c r="E17">
+        <v>11.7417</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4226,8 +5803,14 @@
       <c r="C18">
         <v>9.7036300000000004</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D18">
+        <v>10.474399999999999</v>
+      </c>
+      <c r="E18">
+        <v>10.132400000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4237,8 +5820,14 @@
       <c r="C19">
         <v>13.506600000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D19">
+        <v>12.605</v>
+      </c>
+      <c r="E19">
+        <v>12.171099999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4248,8 +5837,14 @@
       <c r="C20">
         <v>10.099500000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D20">
+        <v>10.0015</v>
+      </c>
+      <c r="E20">
+        <v>10.0015</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4259,8 +5854,14 @@
       <c r="C21">
         <v>9.76431</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D21">
+        <v>11.045500000000001</v>
+      </c>
+      <c r="E21">
+        <v>11.045500000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4270,8 +5871,14 @@
       <c r="C22">
         <v>9.5226299999999995</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D22">
+        <v>10.745200000000001</v>
+      </c>
+      <c r="E22">
+        <v>10.6233</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4281,8 +5888,14 @@
       <c r="C23">
         <v>11.0542</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D23">
+        <v>11.538500000000001</v>
+      </c>
+      <c r="E23">
+        <v>11.538500000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4292,8 +5905,14 @@
       <c r="C24">
         <v>8.6203900000000004</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D24">
+        <v>10.7552</v>
+      </c>
+      <c r="E24">
+        <v>10.628399999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4303,8 +5922,14 @@
       <c r="C25">
         <v>11.9559</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D25">
+        <v>10.5854</v>
+      </c>
+      <c r="E25">
+        <v>10.2044</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4314,8 +5939,14 @@
       <c r="C26">
         <v>9.3543599999999998</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D26">
+        <v>10.4765</v>
+      </c>
+      <c r="E26">
+        <v>10.209300000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4325,8 +5956,14 @@
       <c r="C27">
         <v>10.891400000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D27">
+        <v>11.3018</v>
+      </c>
+      <c r="E27">
+        <v>10.9115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4336,8 +5973,14 @@
       <c r="C28">
         <v>11.9557</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D28">
+        <v>11.8559</v>
+      </c>
+      <c r="E28">
+        <v>11.511799999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4347,8 +5990,14 @@
       <c r="C29">
         <v>8.7629199999999994</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D29">
+        <v>10.3094</v>
+      </c>
+      <c r="E29">
+        <v>10.3094</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4358,8 +6007,14 @@
       <c r="C30">
         <v>8.51478</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D30">
+        <v>11.5632</v>
+      </c>
+      <c r="E30">
+        <v>11.2189</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4369,8 +6024,14 @@
       <c r="C31">
         <v>9.9447100000000006</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D31">
+        <v>11.319599999999999</v>
+      </c>
+      <c r="E31">
+        <v>11.4056</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4380,8 +6041,14 @@
       <c r="C32">
         <v>10.277699999999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D32">
+        <v>14.021100000000001</v>
+      </c>
+      <c r="E32">
+        <v>14.021100000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4391,8 +6058,14 @@
       <c r="C33">
         <v>12.3185</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D33">
+        <v>12.622400000000001</v>
+      </c>
+      <c r="E33">
+        <v>12.5595</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4402,8 +6075,14 @@
       <c r="C34">
         <v>16.7529</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D34">
+        <v>15.266999999999999</v>
+      </c>
+      <c r="E34">
+        <v>15.266999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4413,8 +6092,14 @@
       <c r="C35">
         <v>11.1999</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D35">
+        <v>11.4579</v>
+      </c>
+      <c r="E35">
+        <v>11.1081</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4424,8 +6109,14 @@
       <c r="C36">
         <v>12.0381</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D36">
+        <v>11.7545</v>
+      </c>
+      <c r="E36">
+        <v>11.672800000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4435,8 +6126,14 @@
       <c r="C37">
         <v>7.6860099999999996</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D37">
+        <v>8.38612</v>
+      </c>
+      <c r="E37">
+        <v>8.41615</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4446,8 +6143,14 @@
       <c r="C38">
         <v>8.3811</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D38">
+        <v>9.0785599999999995</v>
+      </c>
+      <c r="E38">
+        <v>9.1180500000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4457,8 +6160,14 @@
       <c r="C39">
         <v>8.0062300000000004</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D39">
+        <v>9.5284399999999998</v>
+      </c>
+      <c r="E39">
+        <v>9.3528599999999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4468,8 +6177,14 @@
       <c r="C40">
         <v>9.0020199999999999</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D40">
+        <v>9.6067499999999999</v>
+      </c>
+      <c r="E40">
+        <v>9.2371400000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4479,8 +6194,14 @@
       <c r="C41">
         <v>8.0299999999999994</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D41">
+        <v>8.5673899999999996</v>
+      </c>
+      <c r="E41">
+        <v>7.7666599999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4490,8 +6211,14 @@
       <c r="C42">
         <v>8.0162600000000008</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D42">
+        <v>8.4891799999999993</v>
+      </c>
+      <c r="E42">
+        <v>7.9642499999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4501,8 +6228,14 @@
       <c r="C43">
         <v>8.7323500000000003</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D43">
+        <v>9.9578799999999994</v>
+      </c>
+      <c r="E43">
+        <v>8.4698399999999996</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4512,8 +6245,14 @@
       <c r="C44">
         <v>7.3470199999999997</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D44">
+        <v>7.5119199999999999</v>
+      </c>
+      <c r="E44">
+        <v>7.0383300000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4523,8 +6262,14 @@
       <c r="C45">
         <v>7.9201300000000003</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D45">
+        <v>7.8134600000000001</v>
+      </c>
+      <c r="E45">
+        <v>7.5830099999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4534,8 +6279,14 @@
       <c r="C46">
         <v>7.8460400000000003</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D46">
+        <v>8.2756399999999992</v>
+      </c>
+      <c r="E46">
+        <v>7.8203800000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4545,8 +6296,14 @@
       <c r="C47">
         <v>10.4794</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D47">
+        <v>10.552899999999999</v>
+      </c>
+      <c r="E47">
+        <v>10.209199999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4556,8 +6313,14 @@
       <c r="C48">
         <v>9.9682099999999991</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D48">
+        <v>10.124499999999999</v>
+      </c>
+      <c r="E48">
+        <v>9.9659999999999993</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4567,8 +6330,14 @@
       <c r="C49">
         <v>13.0229</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D49">
+        <v>13.583399999999999</v>
+      </c>
+      <c r="E49">
+        <v>13.629899999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4578,8 +6347,14 @@
       <c r="C50">
         <v>15.1258</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D50">
+        <v>15.184699999999999</v>
+      </c>
+      <c r="E50">
+        <v>14.894399999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4589,8 +6364,14 @@
       <c r="C51">
         <v>24.1448</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D51">
+        <v>18.245699999999999</v>
+      </c>
+      <c r="E51">
+        <v>18.245699999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4600,8 +6381,14 @@
       <c r="C52">
         <v>18.204599999999999</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D52">
+        <v>22.386500000000002</v>
+      </c>
+      <c r="E52">
+        <v>22.283799999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4613,8 +6400,16 @@
         <f t="array" ref="C53">-inf</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D53" t="e" cm="1">
+        <f t="array" ref="D53">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E53" t="e" cm="1">
+        <f t="array" ref="E53">-inf</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4626,8 +6421,16 @@
         <f t="array" ref="C54">-inf</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D54" t="e" cm="1">
+        <f t="array" ref="D54">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E54" t="e" cm="1">
+        <f t="array" ref="E54">-inf</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4639,8 +6442,16 @@
         <f t="array" ref="C55">-inf</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D55" t="e" cm="1">
+        <f t="array" ref="D55">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E55" t="e" cm="1">
+        <f t="array" ref="E55">-inf</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4651,8 +6462,14 @@
         <f t="array" ref="C56">-inf</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D56">
+        <v>-375.51900000000001</v>
+      </c>
+      <c r="E56">
+        <v>-375.51900000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4664,8 +6481,16 @@
         <f t="array" ref="C57">-inf</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D57" t="e" cm="1">
+        <f t="array" ref="D57">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E57" t="e" cm="1">
+        <f t="array" ref="E57">-inf</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4677,8 +6502,16 @@
         <f t="array" ref="C58">-inf</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D58" t="e" cm="1">
+        <f t="array" ref="D58">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E58" t="e" cm="1">
+        <f t="array" ref="E58">-inf</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4690,8 +6523,16 @@
         <f t="array" ref="C59">-inf</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D59" t="e" cm="1">
+        <f t="array" ref="D59">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E59" t="e" cm="1">
+        <f t="array" ref="E59">-inf</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4703,8 +6544,16 @@
         <f t="array" ref="C60">-inf</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D60" t="e" cm="1">
+        <f t="array" ref="D60">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E60" t="e" cm="1">
+        <f t="array" ref="E60">-inf</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4716,8 +6565,16 @@
         <f t="array" ref="C61">-inf</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D61" t="e" cm="1">
+        <f t="array" ref="D61">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E61" t="e" cm="1">
+        <f t="array" ref="E61">-inf</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4729,8 +6586,16 @@
         <f t="array" ref="C62">-inf</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D62" t="e" cm="1">
+        <f t="array" ref="D62">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E62" t="e" cm="1">
+        <f t="array" ref="E62">-inf</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4742,8 +6607,16 @@
         <f t="array" ref="C63">-inf</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D63" t="e" cm="1">
+        <f t="array" ref="D63">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E63" t="e" cm="1">
+        <f t="array" ref="E63">-inf</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4755,8 +6628,16 @@
         <f t="array" ref="C64">-inf</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D64" t="e" cm="1">
+        <f t="array" ref="D64">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E64" t="e" cm="1">
+        <f t="array" ref="E64">-inf</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4768,8 +6649,16 @@
         <f t="array" ref="C65">-inf</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D65" t="e" cm="1">
+        <f t="array" ref="D65">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E65" t="e" cm="1">
+        <f t="array" ref="E65">-inf</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4781,8 +6670,16 @@
         <f t="array" ref="C66">-inf</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D66" t="e" cm="1">
+        <f t="array" ref="D66">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E66" t="e" cm="1">
+        <f t="array" ref="E66">-inf</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4794,8 +6691,16 @@
         <f t="array" ref="C67">-inf</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D67" t="e" cm="1">
+        <f t="array" ref="D67">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E67" t="e" cm="1">
+        <f t="array" ref="E67">-inf</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4807,8 +6712,16 @@
         <f t="array" ref="C68">-inf</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D68" t="e" cm="1">
+        <f t="array" ref="D68">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E68" t="e" cm="1">
+        <f t="array" ref="E68">-inf</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4820,8 +6733,16 @@
         <f t="array" ref="C69">-inf</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D69" t="e" cm="1">
+        <f t="array" ref="D69">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E69" t="e" cm="1">
+        <f t="array" ref="E69">-inf</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4833,8 +6754,16 @@
         <f t="array" ref="C70">-inf</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D70" t="e" cm="1">
+        <f t="array" ref="D70">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E70" t="e" cm="1">
+        <f t="array" ref="E70">-inf</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4846,8 +6775,16 @@
         <f t="array" ref="C71">-inf</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D71" t="e" cm="1">
+        <f t="array" ref="D71">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E71" t="e" cm="1">
+        <f t="array" ref="E71">-inf</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4859,8 +6796,16 @@
         <f t="array" ref="C72">-inf</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D72" t="e" cm="1">
+        <f t="array" ref="D72">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E72" t="e" cm="1">
+        <f t="array" ref="E72">-inf</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4872,8 +6817,16 @@
         <f t="array" ref="C73">-inf</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D73" t="e" cm="1">
+        <f t="array" ref="D73">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E73" t="e" cm="1">
+        <f t="array" ref="E73">-inf</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4885,8 +6838,16 @@
         <f t="array" ref="C74">-inf</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D74" t="e" cm="1">
+        <f t="array" ref="D74">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E74" t="e" cm="1">
+        <f t="array" ref="E74">-inf</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4898,8 +6859,16 @@
         <f t="array" ref="C75">-inf</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D75" t="e" cm="1">
+        <f t="array" ref="D75">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E75" t="e" cm="1">
+        <f t="array" ref="E75">-inf</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4911,8 +6880,16 @@
         <f t="array" ref="C76">-inf</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D76" t="e" cm="1">
+        <f t="array" ref="D76">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E76" t="e" cm="1">
+        <f t="array" ref="E76">-inf</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4924,8 +6901,16 @@
         <f t="array" ref="C77">-inf</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D77" t="e" cm="1">
+        <f t="array" ref="D77">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E77" t="e" cm="1">
+        <f t="array" ref="E77">-inf</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4935,6 +6920,14 @@
       </c>
       <c r="C78" t="e" cm="1">
         <f t="array" ref="C78">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D78" t="e" cm="1">
+        <f t="array" ref="D78">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E78" t="e" cm="1">
+        <f t="array" ref="E78">-inf</f>
         <v>#NAME?</v>
       </c>
     </row>

</xml_diff>